<commit_message>
LRparse successfully in example 1
</commit_message>
<xml_diff>
--- a/LR parser/parsing table.xlsx
+++ b/LR parser/parsing table.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384DBE6B-F9CF-4172-B405-5122CCC17129}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DD24E7-65B0-4A9F-AE2D-D23C2AC2CC21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="77">
   <si>
     <t>{</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -184,131 +184,135 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>s 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r compoundstmt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r arithexprprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 38</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 39</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r multexprprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r simpleexpr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r assgstmt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r boolop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r arithexpr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r multexpr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 49</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r boolexpr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r whilestmt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 55</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r ifstmt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 57</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r stmt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>s 13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 16</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 17</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r compoundstmt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 22</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 23</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 27</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 29</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 32</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 31</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 33</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 35</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 36</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r arithexprprime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 38</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 39</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r multexprprime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r simpleexpr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r assgstmt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 42</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r boolop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r arithexpr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r multexpr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 49</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r boolexpr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r whilestmt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 55</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r ifstmt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 57</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -645,37 +649,37 @@
   <dimension ref="A1:AL98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="25.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="19" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9" style="2"/>
-    <col min="25" max="25" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -788,7 +792,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -802,7 +806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -810,7 +814,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -818,7 +822,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -856,15 +860,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -902,89 +906,89 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="V8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="V9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="V10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="V11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="M12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="M13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="T14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="W15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -992,18 +996,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="F17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" t="s">
         <v>49</v>
       </c>
-      <c r="G17" t="s">
+      <c r="M17" t="s">
         <v>50</v>
-      </c>
-      <c r="M17" t="s">
-        <v>51</v>
       </c>
       <c r="AF17">
         <v>18</v>
@@ -1018,18 +1022,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="F18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" t="s">
         <v>49</v>
       </c>
-      <c r="G18" t="s">
+      <c r="M18" t="s">
         <v>50</v>
-      </c>
-      <c r="M18" t="s">
-        <v>51</v>
       </c>
       <c r="AF18">
         <v>25</v>
@@ -1044,18 +1048,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="F19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" t="s">
         <v>49</v>
       </c>
-      <c r="G19" t="s">
+      <c r="M19" t="s">
         <v>50</v>
-      </c>
-      <c r="M19" t="s">
-        <v>51</v>
       </c>
       <c r="AH19">
         <v>26</v>
@@ -1067,219 +1071,219 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="O21" t="s">
+        <v>54</v>
+      </c>
+      <c r="P21" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>56</v>
+      </c>
+      <c r="R21" t="s">
         <v>55</v>
       </c>
-      <c r="P21" t="s">
+      <c r="S21" t="s">
         <v>53</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>57</v>
-      </c>
-      <c r="R21" t="s">
-        <v>56</v>
-      </c>
-      <c r="S21" t="s">
-        <v>54</v>
       </c>
       <c r="AG21">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K22" t="s">
+        <v>57</v>
+      </c>
+      <c r="L22" t="s">
         <v>58</v>
       </c>
-      <c r="L22" t="s">
-        <v>59</v>
-      </c>
       <c r="N22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AI22">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I23" t="s">
+        <v>60</v>
+      </c>
+      <c r="J23" t="s">
         <v>61</v>
       </c>
-      <c r="J23" t="s">
-        <v>62</v>
-      </c>
       <c r="K23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AK23">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="M26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AH26">
         <v>40</v>
@@ -1291,42 +1295,42 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="N27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="H28" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="U29" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="F30" t="s">
+        <v>48</v>
+      </c>
+      <c r="G30" t="s">
         <v>49</v>
       </c>
-      <c r="G30" t="s">
+      <c r="M30" t="s">
         <v>50</v>
-      </c>
-      <c r="M30" t="s">
-        <v>51</v>
       </c>
       <c r="AH30">
         <v>42</v>
@@ -1338,120 +1342,120 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="F31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="F32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M32" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="F33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="F34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="F35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V36" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="F37" t="s">
+        <v>48</v>
+      </c>
+      <c r="G37" t="s">
         <v>49</v>
       </c>
-      <c r="G37" t="s">
+      <c r="M37" t="s">
         <v>50</v>
-      </c>
-      <c r="M37" t="s">
-        <v>51</v>
       </c>
       <c r="AJ37">
         <v>44</v>
@@ -1460,90 +1464,90 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="F38" t="s">
+        <v>48</v>
+      </c>
+      <c r="G38" t="s">
         <v>49</v>
       </c>
-      <c r="G38" t="s">
+      <c r="M38" t="s">
         <v>50</v>
-      </c>
-      <c r="M38" t="s">
-        <v>51</v>
       </c>
       <c r="AJ38">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="R39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="F40" t="s">
+        <v>48</v>
+      </c>
+      <c r="G40" t="s">
         <v>49</v>
       </c>
-      <c r="G40" t="s">
+      <c r="M40" t="s">
         <v>50</v>
-      </c>
-      <c r="M40" t="s">
-        <v>51</v>
       </c>
       <c r="AL40">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="F41" t="s">
+        <v>48</v>
+      </c>
+      <c r="G41" t="s">
         <v>49</v>
       </c>
-      <c r="G41" t="s">
+      <c r="M41" t="s">
         <v>50</v>
-      </c>
-      <c r="M41" t="s">
-        <v>51</v>
       </c>
       <c r="AL41">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -1575,15 +1579,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="N43" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -1615,274 +1619,274 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="N45" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="K46" t="s">
+        <v>57</v>
+      </c>
+      <c r="L46" t="s">
         <v>58</v>
-      </c>
-      <c r="L46" t="s">
-        <v>59</v>
       </c>
       <c r="AI46">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="K47" t="s">
+        <v>57</v>
+      </c>
+      <c r="L47" t="s">
         <v>58</v>
-      </c>
-      <c r="L47" t="s">
-        <v>59</v>
       </c>
       <c r="AI47">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="I48" t="s">
+        <v>60</v>
+      </c>
+      <c r="J48" t="s">
         <v>61</v>
-      </c>
-      <c r="J48" t="s">
-        <v>62</v>
       </c>
       <c r="AK48">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="I49" t="s">
+        <v>60</v>
+      </c>
+      <c r="J49" t="s">
         <v>61</v>
-      </c>
-      <c r="J49" t="s">
-        <v>62</v>
       </c>
       <c r="AK49">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="V50" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="V51" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V52" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V53" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V54" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V55" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V56" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -1899,7 +1903,7 @@
         <v>43</v>
       </c>
       <c r="V57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Z57">
         <v>56</v>
@@ -1917,216 +1921,216 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="V59" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
pass 3 in local
</commit_message>
<xml_diff>
--- a/LR parser/parsing table.xlsx
+++ b/LR parser/parsing table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D51C2A-7B14-440E-A31D-899EBD8A17B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C188AAB-817B-41B3-9480-0323331800C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="78">
   <si>
     <t>{</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -313,6 +313,10 @@
   </si>
   <si>
     <t>s 13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 40</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -648,9 +652,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V58" sqref="V58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47:V47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1300,7 +1304,7 @@
         <v>25</v>
       </c>
       <c r="N27" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.25">
@@ -1333,7 +1337,7 @@
         <v>50</v>
       </c>
       <c r="AH30">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AJ30">
         <v>20</v>
@@ -1491,6 +1495,12 @@
       <c r="H39" t="s">
         <v>68</v>
       </c>
+      <c r="K39" t="s">
+        <v>68</v>
+      </c>
+      <c r="L39" t="s">
+        <v>68</v>
+      </c>
       <c r="N39" t="s">
         <v>68</v>
       </c>
@@ -1631,11 +1641,32 @@
       <c r="A46">
         <v>44</v>
       </c>
-      <c r="K46" t="s">
-        <v>57</v>
-      </c>
-      <c r="L46" t="s">
-        <v>58</v>
+      <c r="C46" t="s">
+        <v>59</v>
+      </c>
+      <c r="H46" t="s">
+        <v>59</v>
+      </c>
+      <c r="N46" t="s">
+        <v>59</v>
+      </c>
+      <c r="O46" t="s">
+        <v>59</v>
+      </c>
+      <c r="P46" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>59</v>
+      </c>
+      <c r="R46" t="s">
+        <v>59</v>
+      </c>
+      <c r="S46" t="s">
+        <v>59</v>
+      </c>
+      <c r="V46" t="s">
+        <v>59</v>
       </c>
       <c r="AI46">
         <v>50</v>
@@ -1645,11 +1676,32 @@
       <c r="A47">
         <v>45</v>
       </c>
-      <c r="K47" t="s">
-        <v>57</v>
-      </c>
-      <c r="L47" t="s">
-        <v>58</v>
+      <c r="C47" t="s">
+        <v>59</v>
+      </c>
+      <c r="H47" t="s">
+        <v>59</v>
+      </c>
+      <c r="N47" t="s">
+        <v>59</v>
+      </c>
+      <c r="O47" t="s">
+        <v>59</v>
+      </c>
+      <c r="P47" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>59</v>
+      </c>
+      <c r="R47" t="s">
+        <v>59</v>
+      </c>
+      <c r="S47" t="s">
+        <v>59</v>
+      </c>
+      <c r="V47" t="s">
+        <v>59</v>
       </c>
       <c r="AI47">
         <v>51</v>

</xml_diff>

<commit_message>
pass 4 in local
</commit_message>
<xml_diff>
--- a/LR parser/parsing table.xlsx
+++ b/LR parser/parsing table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BCC1C2-BA37-4CFB-8817-EF5D632088C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DA901B-7164-4061-8579-3DDE4C476D4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="80">
   <si>
     <t>{</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -212,111 +212,119 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>s 29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 36</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r arithexprprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 38</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 39</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r multexprprime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r simpleexpr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r assgstmt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 42</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r boolop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r arithexpr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r multexpr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 49</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r boolexpr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r whilestmt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 55</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r ifstmt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 57</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r stmt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s 40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>s 27</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>s 29</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 32</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 31</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 33</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 35</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 36</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r arithexprprime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>s 38</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>s 39</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r multexprprime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r simpleexpr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r assgstmt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 42</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r boolop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r arithexpr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r multexpr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 49</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r boolexpr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r whilestmt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 55</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r ifstmt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 57</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r stmt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s 40</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -652,9 +660,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK49" sqref="AK49"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -869,7 +877,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
@@ -915,10 +923,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="V8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
@@ -926,10 +934,10 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="V9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
@@ -937,10 +945,10 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="V10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
@@ -948,10 +956,10 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="V11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
@@ -1079,8 +1087,8 @@
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="C20" t="s">
-        <v>51</v>
+      <c r="N20" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.25">
@@ -1088,19 +1096,19 @@
         <v>19</v>
       </c>
       <c r="O21" t="s">
+        <v>53</v>
+      </c>
+      <c r="P21" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>55</v>
+      </c>
+      <c r="R21" t="s">
         <v>54</v>
       </c>
-      <c r="P21" t="s">
+      <c r="S21" t="s">
         <v>52</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>56</v>
-      </c>
-      <c r="R21" t="s">
-        <v>55</v>
-      </c>
-      <c r="S21" t="s">
-        <v>53</v>
       </c>
       <c r="AG21">
         <v>28</v>
@@ -1111,37 +1119,37 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K22" t="s">
+        <v>56</v>
+      </c>
+      <c r="L22" t="s">
         <v>57</v>
       </c>
-      <c r="L22" t="s">
-        <v>58</v>
-      </c>
       <c r="N22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI22">
         <v>34</v>
@@ -1152,43 +1160,43 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I23" t="s">
+        <v>59</v>
+      </c>
+      <c r="J23" t="s">
         <v>60</v>
       </c>
-      <c r="J23" t="s">
-        <v>61</v>
-      </c>
       <c r="K23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AK23">
         <v>37</v>
@@ -1199,43 +1207,43 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.25">
@@ -1243,43 +1251,43 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.25">
@@ -1304,7 +1312,7 @@
         <v>25</v>
       </c>
       <c r="N27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.25">
@@ -1312,7 +1320,7 @@
         <v>26</v>
       </c>
       <c r="H28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.25">
@@ -1320,7 +1328,7 @@
         <v>27</v>
       </c>
       <c r="U29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.25">
@@ -1351,13 +1359,13 @@
         <v>29</v>
       </c>
       <c r="F31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.25">
@@ -1365,13 +1373,13 @@
         <v>30</v>
       </c>
       <c r="F32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.25">
@@ -1379,13 +1387,13 @@
         <v>31</v>
       </c>
       <c r="F33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.25">
@@ -1393,13 +1401,13 @@
         <v>32</v>
       </c>
       <c r="F34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.25">
@@ -1407,13 +1415,13 @@
         <v>33</v>
       </c>
       <c r="F35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.25">
@@ -1421,31 +1429,31 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="V36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.25">
@@ -1490,37 +1498,37 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:38" x14ac:dyDescent="0.25">
@@ -1594,7 +1602,7 @@
         <v>41</v>
       </c>
       <c r="N43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:38" x14ac:dyDescent="0.25">
@@ -1634,7 +1642,7 @@
         <v>43</v>
       </c>
       <c r="N45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.25">
@@ -1642,31 +1650,31 @@
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI46">
         <v>51</v>
@@ -1677,31 +1685,31 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI47">
         <v>52</v>
@@ -1711,10 +1719,43 @@
       <c r="A48">
         <v>46</v>
       </c>
+      <c r="C48" t="s">
+        <v>61</v>
+      </c>
+      <c r="H48" t="s">
+        <v>61</v>
+      </c>
       <c r="I48" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="J48" t="s">
+        <v>79</v>
+      </c>
+      <c r="K48" t="s">
+        <v>61</v>
+      </c>
+      <c r="L48" t="s">
+        <v>61</v>
+      </c>
+      <c r="N48" t="s">
+        <v>61</v>
+      </c>
+      <c r="O48" t="s">
+        <v>61</v>
+      </c>
+      <c r="P48" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>61</v>
+      </c>
+      <c r="R48" t="s">
+        <v>61</v>
+      </c>
+      <c r="S48" t="s">
+        <v>61</v>
+      </c>
+      <c r="V48" t="s">
         <v>61</v>
       </c>
       <c r="AK48">
@@ -1725,10 +1766,43 @@
       <c r="A49">
         <v>47</v>
       </c>
+      <c r="C49" t="s">
+        <v>61</v>
+      </c>
+      <c r="H49" t="s">
+        <v>61</v>
+      </c>
       <c r="I49" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="J49" t="s">
+        <v>79</v>
+      </c>
+      <c r="K49" t="s">
+        <v>61</v>
+      </c>
+      <c r="L49" t="s">
+        <v>61</v>
+      </c>
+      <c r="N49" t="s">
+        <v>61</v>
+      </c>
+      <c r="O49" t="s">
+        <v>61</v>
+      </c>
+      <c r="P49" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>61</v>
+      </c>
+      <c r="R49" t="s">
+        <v>61</v>
+      </c>
+      <c r="S49" t="s">
+        <v>61</v>
+      </c>
+      <c r="V49" t="s">
         <v>61</v>
       </c>
       <c r="AK49">
@@ -1740,10 +1814,10 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:37" x14ac:dyDescent="0.25">
@@ -1751,7 +1825,7 @@
         <v>49</v>
       </c>
       <c r="V51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:37" x14ac:dyDescent="0.25">
@@ -1759,43 +1833,43 @@
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:37" x14ac:dyDescent="0.25">
@@ -1803,31 +1877,31 @@
         <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:37" x14ac:dyDescent="0.25">
@@ -1835,31 +1909,31 @@
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:37" x14ac:dyDescent="0.25">
@@ -1867,37 +1941,37 @@
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:37" x14ac:dyDescent="0.25">
@@ -1905,37 +1979,37 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:37" x14ac:dyDescent="0.25">
@@ -1975,10 +2049,10 @@
         <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:37" x14ac:dyDescent="0.25">
@@ -1986,10 +2060,10 @@
         <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>